<commit_message>
Facebook Selenium Automation test
</commit_message>
<xml_diff>
--- a/STD_Facebook_Website.xlsx
+++ b/STD_Facebook_Website.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Videos\my hightech file\Project\Project3-selelinum\Selinum\Facebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C49896-1428-4B67-86EA-FA87CE77C16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4319D86-8ABC-4602-BBF7-0AD5B44FB116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{7D02D6C4-F827-43B6-9C77-530AA849038B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="154">
   <si>
     <t xml:space="preserve">Google Chrome Web will be open </t>
   </si>
@@ -608,9 +608,6 @@
     <t>FBL005</t>
   </si>
   <si>
-    <t>FBL006</t>
-  </si>
-  <si>
     <t>FBF001</t>
   </si>
   <si>
@@ -722,6 +719,51 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "You use this when you log in and if you ever need to reset your password"</t>
+    </r>
+  </si>
+  <si>
+    <t>FBL004</t>
+  </si>
+  <si>
+    <t>FBF003</t>
+  </si>
+  <si>
+    <t>FBS0006</t>
+  </si>
+  <si>
+    <t>Last Name will be blank</t>
+  </si>
+  <si>
+    <t>Last Name field will be blank</t>
+  </si>
+  <si>
+    <t>Test Facebook Validate Registering with Null Last Name</t>
+  </si>
+  <si>
+    <t>FBS0007</t>
+  </si>
+  <si>
+    <t>Blank Birth Date</t>
+  </si>
+  <si>
+    <t>BirthDay Field will be blank</t>
+  </si>
+  <si>
+    <t>Test Facebook Validate Registering with Null Birth day</t>
+  </si>
+  <si>
+    <r>
+      <t>Display Error Message</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "It looks like you enter wrong info"</t>
     </r>
   </si>
 </sst>
@@ -1114,7 +1156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1175,11 +1217,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1202,26 +1259,76 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1785,8 +1892,8 @@
   </sheetPr>
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82:C82"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B84" sqref="B84:C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1800,97 +1907,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="35"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="34"/>
+      <c r="C4" s="39"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="30"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="30"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="28"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="27"/>
+      <c r="C8" s="30"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="30"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="27"/>
+      <c r="C10" s="30"/>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38"/>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="32"/>
+      <c r="B11" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="30"/>
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
@@ -2005,97 +2112,97 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="35"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="C21" s="32"/>
+      <c r="C21" s="37"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="27"/>
+      <c r="C22" s="30"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="34"/>
+      <c r="C23" s="39"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="27"/>
+      <c r="C24" s="30"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="27"/>
+      <c r="C25" s="30"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="36"/>
+      <c r="C26" s="28"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="27"/>
+      <c r="C27" s="30"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="27"/>
+      <c r="C28" s="30"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="38"/>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="32"/>
+      <c r="B29" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="27"/>
+      <c r="C29" s="30"/>
     </row>
     <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="38"/>
-      <c r="B30" s="26" t="s">
+      <c r="A30" s="32"/>
+      <c r="B30" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="27"/>
+      <c r="C30" s="30"/>
     </row>
     <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
@@ -2211,97 +2318,97 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="30"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="35"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="C40" s="32"/>
+      <c r="C40" s="37"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="27"/>
+      <c r="C41" s="30"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="34"/>
+      <c r="C42" s="39"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="27"/>
+      <c r="C43" s="30"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="27"/>
+      <c r="C44" s="30"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="36"/>
+      <c r="C45" s="28"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="27"/>
+      <c r="C46" s="30"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="37" t="s">
+      <c r="A47" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C47" s="27"/>
+      <c r="C47" s="30"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="38"/>
-      <c r="B48" s="26" t="s">
+      <c r="A48" s="32"/>
+      <c r="B48" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="27"/>
+      <c r="C48" s="30"/>
     </row>
     <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="38"/>
-      <c r="B49" s="26" t="s">
+      <c r="A49" s="32"/>
+      <c r="B49" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="27"/>
+      <c r="C49" s="30"/>
     </row>
     <row r="50" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="18" t="s">
@@ -2416,97 +2523,97 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="29"/>
-      <c r="C58" s="30"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="35"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B59" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="C59" s="32"/>
+      <c r="B59" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C59" s="37"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B60" s="26" t="s">
+      <c r="B60" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="27"/>
+      <c r="C60" s="30"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B61" s="33" t="s">
+      <c r="B61" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C61" s="34"/>
+      <c r="C61" s="39"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B62" s="26" t="s">
+      <c r="B62" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C62" s="27"/>
+      <c r="C62" s="30"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B63" s="26" t="s">
+      <c r="B63" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C63" s="27"/>
+      <c r="C63" s="30"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B64" s="35" t="s">
+      <c r="B64" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="36"/>
+      <c r="C64" s="28"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B65" s="26" t="s">
+      <c r="B65" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C65" s="27"/>
+      <c r="C65" s="30"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="37" t="s">
+      <c r="A66" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="26" t="s">
+      <c r="B66" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C66" s="27"/>
+      <c r="C66" s="30"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="38"/>
-      <c r="B67" s="26" t="s">
+      <c r="A67" s="32"/>
+      <c r="B67" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C67" s="27"/>
+      <c r="C67" s="30"/>
     </row>
     <row r="68" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="38"/>
-      <c r="B68" s="26" t="s">
+      <c r="A68" s="32"/>
+      <c r="B68" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C68" s="27"/>
+      <c r="C68" s="30"/>
     </row>
     <row r="69" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="18" t="s">
@@ -2621,97 +2728,97 @@
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A77" s="28" t="s">
+      <c r="A77" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B77" s="29"/>
-      <c r="C77" s="30"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="35"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B78" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="C78" s="32"/>
+      <c r="B78" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C78" s="37"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B79" s="26" t="s">
+      <c r="B79" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C79" s="27"/>
+      <c r="C79" s="30"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B80" s="33" t="s">
+      <c r="B80" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C80" s="34"/>
+      <c r="C80" s="39"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="26" t="s">
+      <c r="B81" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C81" s="27"/>
+      <c r="C81" s="30"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B82" s="26" t="s">
+      <c r="B82" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="27"/>
+      <c r="C82" s="30"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B83" s="35" t="s">
+      <c r="B83" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C83" s="36"/>
+      <c r="C83" s="28"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B84" s="26" t="s">
+      <c r="B84" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C84" s="27"/>
+      <c r="C84" s="30"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="37" t="s">
+      <c r="A85" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B85" s="26" t="s">
+      <c r="B85" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C85" s="27"/>
+      <c r="C85" s="30"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="38"/>
-      <c r="B86" s="26" t="s">
+      <c r="A86" s="32"/>
+      <c r="B86" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C86" s="27"/>
+      <c r="C86" s="30"/>
     </row>
     <row r="87" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="38"/>
-      <c r="B87" s="26" t="s">
+      <c r="A87" s="32"/>
+      <c r="B87" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C87" s="27"/>
+      <c r="C87" s="30"/>
     </row>
     <row r="88" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="18" t="s">
@@ -2799,12 +2906,48 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
     <mergeCell ref="B82:C82"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B65:C65"/>
@@ -2817,90 +2960,54 @@
     <mergeCell ref="B79:C79"/>
     <mergeCell ref="B80:C80"/>
     <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
   </mergeCells>
   <conditionalFormatting sqref="D12:D18 D88:D92">
-    <cfRule type="containsBlanks" dxfId="23" priority="13">
+    <cfRule type="containsBlanks" dxfId="29" priority="13">
       <formula>LEN(TRIM(D12))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="V">
+    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="V">
       <formula>NOT(ISERROR(SEARCH("V",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D37">
-    <cfRule type="containsBlanks" dxfId="20" priority="10">
+    <cfRule type="containsBlanks" dxfId="26" priority="10">
       <formula>LEN(TRIM(D31))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="11" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="V">
+    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="V">
       <formula>NOT(ISERROR(SEARCH("V",D31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50:D56">
-    <cfRule type="containsBlanks" dxfId="17" priority="7">
+    <cfRule type="containsBlanks" dxfId="23" priority="7">
       <formula>LEN(TRIM(D50))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="V">
+    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="V">
       <formula>NOT(ISERROR(SEARCH("V",D50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:D75">
-    <cfRule type="containsBlanks" dxfId="14" priority="4">
+    <cfRule type="containsBlanks" dxfId="20" priority="4">
       <formula>LEN(TRIM(D69))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D69)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="V">
+    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="V">
       <formula>NOT(ISERROR(SEARCH("V",D69)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2916,8 +3023,8 @@
   </sheetPr>
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2931,97 +3038,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="35"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="32"/>
+      <c r="B2" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="34"/>
+      <c r="C4" s="39"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="30"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="30"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="28"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="27"/>
+      <c r="C8" s="30"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="30"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="27"/>
+      <c r="C10" s="30"/>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38"/>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="32"/>
+      <c r="B11" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="30"/>
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
@@ -3276,97 +3383,97 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="30"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="C31" s="32"/>
+      <c r="B31" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="37"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" s="27"/>
+      <c r="B32" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="30"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="34"/>
+      <c r="C33" s="39"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="27"/>
+      <c r="C34" s="30"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="27"/>
+      <c r="C35" s="30"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="36"/>
+      <c r="C36" s="28"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="27"/>
+      <c r="C37" s="30"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="27"/>
+      <c r="C38" s="30"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="38"/>
-      <c r="B39" s="26" t="s">
+      <c r="A39" s="32"/>
+      <c r="B39" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="27"/>
+      <c r="C39" s="30"/>
     </row>
     <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="38"/>
-      <c r="B40" s="26" t="s">
+      <c r="A40" s="32"/>
+      <c r="B40" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="27"/>
+      <c r="C40" s="30"/>
     </row>
     <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="18" t="s">
@@ -3466,7 +3573,7 @@
         <v>104</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="1"/>
@@ -3495,97 +3602,97 @@
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="28" t="s">
+      <c r="A50" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="30"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="35"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="C51" s="32"/>
+      <c r="B51" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="37"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B52" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="C52" s="27"/>
+      <c r="B52" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52" s="30"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="33" t="s">
+      <c r="B53" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="34"/>
+      <c r="C53" s="39"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="26" t="s">
+      <c r="B54" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="27"/>
+      <c r="C54" s="30"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="26" t="s">
+      <c r="B55" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="27"/>
+      <c r="C55" s="30"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B56" s="35" t="s">
+      <c r="B56" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="36"/>
+      <c r="C56" s="28"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B57" s="26" t="s">
+      <c r="B57" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C57" s="27"/>
+      <c r="C57" s="30"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="37" t="s">
+      <c r="A58" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B58" s="26" t="s">
+      <c r="B58" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C58" s="27"/>
+      <c r="C58" s="30"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="38"/>
-      <c r="B59" s="26" t="s">
+      <c r="A59" s="32"/>
+      <c r="B59" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C59" s="27"/>
+      <c r="C59" s="30"/>
     </row>
     <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="38"/>
-      <c r="B60" s="26" t="s">
+      <c r="A60" s="32"/>
+      <c r="B60" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C60" s="27"/>
+      <c r="C60" s="30"/>
     </row>
     <row r="61" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="18" t="s">
@@ -3671,7 +3778,7 @@
         <v>104</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="1"/>
@@ -3701,18 +3808,23 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B57:C57"/>
@@ -3720,43 +3832,38 @@
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B58:C58"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <conditionalFormatting sqref="D12:D28 D61:D67">
-    <cfRule type="containsBlanks" dxfId="11" priority="16">
+    <cfRule type="containsBlanks" dxfId="17" priority="16">
       <formula>LEN(TRIM(D12))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="V">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="V">
       <formula>NOT(ISERROR(SEARCH("V",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41:D48">
-    <cfRule type="containsBlanks" dxfId="8" priority="4">
+    <cfRule type="containsBlanks" dxfId="14" priority="4">
       <formula>LEN(TRIM(D41))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="V">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="V">
       <formula>NOT(ISERROR(SEARCH("V",D41)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3770,10 +3877,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3787,97 +3894,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="35"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="34"/>
+      <c r="C4" s="39"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="30"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="30"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="28"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="27"/>
+      <c r="C8" s="30"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="30"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="27"/>
+      <c r="C10" s="30"/>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38"/>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="32"/>
+      <c r="B11" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="30"/>
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
@@ -4188,97 +4295,97 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="29"/>
-      <c r="C34" s="30"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="32"/>
+      <c r="C35" s="37"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="27"/>
+      <c r="C36" s="30"/>
     </row>
     <row r="37" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="33" t="s">
+      <c r="B37" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="34"/>
+      <c r="C37" s="39"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="27"/>
+      <c r="C38" s="30"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="27"/>
+      <c r="C39" s="30"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="36"/>
+      <c r="C40" s="28"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="27"/>
+      <c r="C41" s="30"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="27"/>
+      <c r="C42" s="30"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="38"/>
-      <c r="B43" s="26" t="s">
+      <c r="A43" s="32"/>
+      <c r="B43" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="27"/>
+      <c r="C43" s="30"/>
     </row>
     <row r="44" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="38"/>
-      <c r="B44" s="26" t="s">
+      <c r="A44" s="32"/>
+      <c r="B44" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="27"/>
+      <c r="C44" s="30"/>
     </row>
     <row r="45" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="18" t="s">
@@ -4364,7 +4471,7 @@
         <v>74</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="1"/>
@@ -4393,97 +4500,97 @@
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="28" t="s">
+      <c r="A53" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="30"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="35"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="31" t="s">
+      <c r="B54" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="32"/>
+      <c r="C54" s="37"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="26" t="s">
+      <c r="B55" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="27"/>
+      <c r="C55" s="30"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B56" s="33" t="s">
+      <c r="B56" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="C56" s="34"/>
+      <c r="C56" s="39"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B57" s="26" t="s">
+      <c r="B57" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="27"/>
+      <c r="C57" s="30"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="26" t="s">
+      <c r="B58" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C58" s="27"/>
+      <c r="C58" s="30"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B59" s="35" t="s">
+      <c r="B59" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="36"/>
+      <c r="C59" s="28"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B60" s="26" t="s">
+      <c r="B60" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="27"/>
+      <c r="C60" s="30"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="37" t="s">
+      <c r="A61" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B61" s="26" t="s">
+      <c r="B61" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C61" s="27"/>
+      <c r="C61" s="30"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="38"/>
-      <c r="B62" s="26" t="s">
+      <c r="A62" s="32"/>
+      <c r="B62" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C62" s="27"/>
+      <c r="C62" s="30"/>
     </row>
     <row r="63" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="38"/>
-      <c r="B63" s="26" t="s">
+      <c r="A63" s="32"/>
+      <c r="B63" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C63" s="27"/>
+      <c r="C63" s="30"/>
     </row>
     <row r="64" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="18" t="s">
@@ -4695,7 +4802,7 @@
         <v>74</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="1"/>
@@ -4724,97 +4831,97 @@
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A81" s="28" t="s">
+      <c r="A81" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B81" s="29"/>
-      <c r="C81" s="30"/>
+      <c r="B81" s="34"/>
+      <c r="C81" s="35"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B82" s="31" t="s">
+      <c r="B82" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="C82" s="32"/>
+      <c r="C82" s="37"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B83" s="26" t="s">
+      <c r="B83" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C83" s="27"/>
+      <c r="C83" s="30"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B84" s="33" t="s">
+      <c r="B84" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="C84" s="34"/>
+      <c r="C84" s="39"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B85" s="26" t="s">
+      <c r="B85" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C85" s="27"/>
+      <c r="C85" s="30"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B86" s="26" t="s">
+      <c r="B86" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C86" s="27"/>
+      <c r="C86" s="30"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B87" s="35" t="s">
+      <c r="B87" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C87" s="36"/>
+      <c r="C87" s="28"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B88" s="26" t="s">
+      <c r="B88" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C88" s="27"/>
+      <c r="C88" s="30"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="37" t="s">
+      <c r="A89" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B89" s="26" t="s">
+      <c r="B89" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C89" s="27"/>
+      <c r="C89" s="30"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="38"/>
-      <c r="B90" s="26" t="s">
+      <c r="A90" s="32"/>
+      <c r="B90" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C90" s="27"/>
+      <c r="C90" s="30"/>
     </row>
     <row r="91" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="38"/>
-      <c r="B91" s="26" t="s">
+      <c r="A91" s="32"/>
+      <c r="B91" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C91" s="27"/>
+      <c r="C91" s="30"/>
     </row>
     <row r="92" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="18" t="s">
@@ -5008,11 +5115,11 @@
       <c r="A105" s="7">
         <v>13</v>
       </c>
-      <c r="B105" s="39" t="s">
+      <c r="B105" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C105" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="C105" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="1"/>
@@ -5026,7 +5133,7 @@
         <v>74</v>
       </c>
       <c r="C106" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="1"/>
@@ -5055,97 +5162,97 @@
       <c r="F108" s="1"/>
     </row>
     <row r="109" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A109" s="28" t="s">
+      <c r="A109" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B109" s="29"/>
-      <c r="C109" s="30"/>
+      <c r="B109" s="34"/>
+      <c r="C109" s="35"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B110" s="31" t="s">
+      <c r="B110" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="C110" s="32"/>
+      <c r="C110" s="37"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B111" s="26" t="s">
+      <c r="B111" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="C111" s="27"/>
+      <c r="C111" s="30"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B112" s="33" t="s">
+      <c r="B112" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="C112" s="34"/>
+      <c r="C112" s="39"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B113" s="26" t="s">
+      <c r="B113" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C113" s="27"/>
+      <c r="C113" s="30"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B114" s="26" t="s">
+      <c r="B114" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C114" s="27"/>
+      <c r="C114" s="30"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B115" s="35" t="s">
+      <c r="B115" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C115" s="36"/>
+      <c r="C115" s="28"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B116" s="26" t="s">
+      <c r="B116" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C116" s="27"/>
+      <c r="C116" s="30"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="37" t="s">
+      <c r="A117" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B117" s="26" t="s">
+      <c r="B117" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C117" s="27"/>
+      <c r="C117" s="30"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="38"/>
-      <c r="B118" s="26" t="s">
+      <c r="A118" s="32"/>
+      <c r="B118" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C118" s="27"/>
+      <c r="C118" s="30"/>
     </row>
     <row r="119" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="38"/>
-      <c r="B119" s="26" t="s">
+      <c r="A119" s="32"/>
+      <c r="B119" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C119" s="27"/>
+      <c r="C119" s="30"/>
     </row>
     <row r="120" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="18" t="s">
@@ -5227,11 +5334,11 @@
       <c r="A125" s="7">
         <v>5</v>
       </c>
-      <c r="B125" s="39" t="s">
+      <c r="B125" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C125" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="C125" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="1"/>
@@ -5357,7 +5464,7 @@
         <v>74</v>
       </c>
       <c r="C134" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="1"/>
@@ -5377,7 +5484,7 @@
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="3"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -5385,53 +5492,694 @@
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
     </row>
+    <row r="137" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A137" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B137" s="34"/>
+      <c r="C137" s="35"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B138" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C138" s="37"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B139" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="C139" s="30"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B140" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C140" s="39"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B141" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C141" s="30"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A142" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B142" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C142" s="30"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B143" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C143" s="28"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B144" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C144" s="30"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B145" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C145" s="30"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" s="32"/>
+      <c r="B146" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C146" s="30"/>
+    </row>
+    <row r="147" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A147" s="32"/>
+      <c r="B147" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C147" s="30"/>
+    </row>
+    <row r="148" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A148" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B148" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D148" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E148" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F148" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149" s="12">
+        <v>1</v>
+      </c>
+      <c r="B149" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C149" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D149" s="4"/>
+      <c r="E149" s="1"/>
+      <c r="F149" s="1"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150" s="7">
+        <v>2</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C150" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D150" s="4"/>
+      <c r="E150" s="1"/>
+      <c r="F150" s="1"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151" s="22">
+        <v>3</v>
+      </c>
+      <c r="B151" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C151" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D151" s="4"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" s="7">
+        <v>4</v>
+      </c>
+      <c r="B152" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C152" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D152" s="4"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="1"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" s="7">
+        <v>5</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D153" s="4"/>
+      <c r="E153" s="1"/>
+      <c r="F153" s="1"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" s="22">
+        <v>6</v>
+      </c>
+      <c r="B154" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D154" s="4"/>
+      <c r="E154" s="1"/>
+      <c r="F154" s="1"/>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" s="7">
+        <v>7</v>
+      </c>
+      <c r="B155" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D155" s="4"/>
+      <c r="E155" s="1"/>
+      <c r="F155" s="1"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" s="7">
+        <v>8</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C156" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D156" s="4"/>
+      <c r="E156" s="1"/>
+      <c r="F156" s="1"/>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" s="22">
+        <v>9</v>
+      </c>
+      <c r="B157" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D157" s="4"/>
+      <c r="E157" s="1"/>
+      <c r="F157" s="1"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" s="7">
+        <v>10</v>
+      </c>
+      <c r="B158" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D158" s="4"/>
+      <c r="E158" s="1"/>
+      <c r="F158" s="1"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" s="7">
+        <v>11</v>
+      </c>
+      <c r="B159" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C159" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D159" s="4"/>
+      <c r="E159" s="1"/>
+      <c r="F159" s="1"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" s="22">
+        <v>12</v>
+      </c>
+      <c r="B160" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D160" s="4"/>
+      <c r="E160" s="1"/>
+      <c r="F160" s="1"/>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" s="7">
+        <v>13</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D161" s="4"/>
+      <c r="E161" s="1"/>
+      <c r="F161" s="1"/>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" s="7">
+        <v>14</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C162" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="D162" s="4"/>
+      <c r="E162" s="1"/>
+      <c r="F162" s="1"/>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" s="22">
+        <v>15</v>
+      </c>
+      <c r="B163" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C163" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D163" s="4"/>
+      <c r="E163" s="1"/>
+      <c r="F163" s="1"/>
+    </row>
+    <row r="164" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="3"/>
+      <c r="B164" s="2"/>
+      <c r="C164" s="2"/>
+      <c r="D164" s="1"/>
+      <c r="E164" s="1"/>
+      <c r="F164" s="1"/>
+    </row>
+    <row r="165" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A165" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B165" s="34"/>
+      <c r="C165" s="35"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B166" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C166" s="37"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B167" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="C167" s="30"/>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B168" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C168" s="39"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B169" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C169" s="30"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B170" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C170" s="30"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B171" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C171" s="28"/>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A172" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B172" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C172" s="30"/>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A173" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B173" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C173" s="30"/>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A174" s="32"/>
+      <c r="B174" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C174" s="30"/>
+    </row>
+    <row r="175" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A175" s="32"/>
+      <c r="B175" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C175" s="30"/>
+    </row>
+    <row r="176" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A176" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B176" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C176" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D176" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E176" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F176" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A177" s="12">
+        <v>1</v>
+      </c>
+      <c r="B177" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C177" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D177" s="4"/>
+      <c r="E177" s="1"/>
+      <c r="F177" s="1"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A178" s="7">
+        <v>2</v>
+      </c>
+      <c r="B178" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C178" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D178" s="4"/>
+      <c r="E178" s="1"/>
+      <c r="F178" s="1"/>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179" s="22">
+        <v>3</v>
+      </c>
+      <c r="B179" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C179" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D179" s="4"/>
+      <c r="E179" s="1"/>
+      <c r="F179" s="1"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A180" s="7">
+        <v>4</v>
+      </c>
+      <c r="B180" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C180" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D180" s="4"/>
+      <c r="E180" s="1"/>
+      <c r="F180" s="1"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A181" s="7">
+        <v>5</v>
+      </c>
+      <c r="B181" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C181" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D181" s="4"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="1"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A182" s="22">
+        <v>6</v>
+      </c>
+      <c r="B182" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C182" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D182" s="4"/>
+      <c r="E182" s="1"/>
+      <c r="F182" s="1"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A183" s="7">
+        <v>7</v>
+      </c>
+      <c r="B183" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C183" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D183" s="4"/>
+      <c r="E183" s="1"/>
+      <c r="F183" s="1"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A184" s="7">
+        <v>8</v>
+      </c>
+      <c r="B184" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C184" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D184" s="4"/>
+      <c r="E184" s="1"/>
+      <c r="F184" s="1"/>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A185" s="22">
+        <v>9</v>
+      </c>
+      <c r="B185" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C185" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D185" s="4"/>
+      <c r="E185" s="1"/>
+      <c r="F185" s="1"/>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A186" s="7">
+        <v>10</v>
+      </c>
+      <c r="B186" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C186" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="D186" s="4"/>
+      <c r="E186" s="1"/>
+      <c r="F186" s="1"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A187" s="7">
+        <v>11</v>
+      </c>
+      <c r="B187" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C187" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D187" s="4"/>
+      <c r="E187" s="1"/>
+      <c r="F187" s="1"/>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A188" s="22">
+        <v>12</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C188" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D188" s="4"/>
+      <c r="E188" s="1"/>
+      <c r="F188" s="1"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A189" s="7">
+        <v>13</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D189" s="4"/>
+      <c r="E189" s="1"/>
+      <c r="F189" s="1"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A190" s="7">
+        <v>14</v>
+      </c>
+      <c r="B190" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C190" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D190" s="4"/>
+      <c r="E190" s="1"/>
+      <c r="F190" s="1"/>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A191" s="22">
+        <v>15</v>
+      </c>
+      <c r="B191" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C191" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D191" s="4"/>
+      <c r="E191" s="1"/>
+      <c r="F191" s="1"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A192" s="3"/>
+      <c r="B192" s="2"/>
+      <c r="C192" s="2"/>
+      <c r="D192" s="1"/>
+      <c r="E192" s="1"/>
+      <c r="F192" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="A117:A119"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="A109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B113:C113"/>
+  <mergeCells count="84">
+    <mergeCell ref="B170:C170"/>
+    <mergeCell ref="B171:C171"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="A173:A175"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="B175:C175"/>
+    <mergeCell ref="A165:C165"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="B169:C169"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="A137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="B141:C141"/>
     <mergeCell ref="B114:C114"/>
     <mergeCell ref="B87:C87"/>
     <mergeCell ref="B88:C88"/>
@@ -5447,27 +6195,94 @@
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
+    <mergeCell ref="A109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="A117:A119"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <conditionalFormatting sqref="D12:D32 D45:D51 D92:D107 D120:D135">
-    <cfRule type="containsBlanks" dxfId="5" priority="13">
+    <cfRule type="containsBlanks" dxfId="11" priority="19">
       <formula>LEN(TRIM(D12))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="10" priority="20" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="V">
+    <cfRule type="containsText" dxfId="9" priority="21" operator="containsText" text="V">
       <formula>NOT(ISERROR(SEARCH("V",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64:D79">
-    <cfRule type="containsBlanks" dxfId="2" priority="10">
+    <cfRule type="containsBlanks" dxfId="8" priority="16">
       <formula>LEN(TRIM(D64))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="7" priority="17" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="12" operator="containsText" text="V">
+    <cfRule type="containsText" dxfId="6" priority="18" operator="containsText" text="V">
       <formula>NOT(ISERROR(SEARCH("V",D64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D148:D163">
+    <cfRule type="containsBlanks" dxfId="5" priority="4">
+      <formula>LEN(TRIM(D148))=0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",D148)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="V">
+      <formula>NOT(ISERROR(SEARCH("V",D148)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D176:D191">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
+      <formula>LEN(TRIM(D176))=0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",D176)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="V">
+      <formula>NOT(ISERROR(SEARCH("V",D176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>